<commit_message>
Checked the data for fish species
</commit_message>
<xml_diff>
--- a/Data/Master/Fish species_Initial Check.xlsx
+++ b/Data/Master/Fish species_Initial Check.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louwclaassens/Documents/WorldFish/Ikan Ba Futura_2023/Science and colabs/Ecological Modeling/Timor-Leste South Coast/Timor_South_Ecopath/Timor_Ecopath/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louwclaassens/Documents/WorldFish/Ikan Ba Futura_2023/Science and colabs/Ecological Modeling/Timor-Leste South Coast/Timor_South_Ecopath/Timor_Ecopath/Data/Master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D633117-A3F5-CA40-B25C-9DF13A3A09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485D58B-6AEA-E149-827F-712753CBC5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="680" windowWidth="28040" windowHeight="16780" xr2:uid="{8B661F92-5076-464D-8422-0F08A21EB7CC}"/>
   </bookViews>
@@ -2862,7 +2862,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D43BBC-FD48-6D4B-B79D-D054E095EE14}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2945,7 +2944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -3092,7 +3091,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -3180,7 +3179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>17</v>
       </c>
@@ -3323,7 +3322,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -3415,7 +3414,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
@@ -3450,7 +3449,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -3499,7 +3498,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
@@ -3595,7 +3594,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>6</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>6</v>
       </c>
@@ -3724,7 +3723,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
@@ -4006,7 +4005,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
@@ -4053,7 +4052,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -4098,7 +4097,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>162</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -4237,7 +4236,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
@@ -4282,7 +4281,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>6</v>
       </c>
@@ -4372,7 +4371,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="1:17" ht="221" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="221" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>6</v>
       </c>
@@ -4421,7 +4420,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="204" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="204" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -4564,7 +4563,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
@@ -4599,7 +4598,7 @@
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>6</v>
       </c>
@@ -4644,7 +4643,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>6</v>
       </c>
@@ -4689,7 +4688,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>6</v>
       </c>
@@ -4736,7 +4735,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>51</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>51</v>
       </c>
@@ -4824,7 +4823,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>17</v>
       </c>
@@ -4871,7 +4870,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>17</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>57</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>206</v>
       </c>
@@ -5062,7 +5061,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>59</v>
       </c>
@@ -5109,7 +5108,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>61</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>63</v>
       </c>
@@ -5211,7 +5210,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>66</v>
       </c>
@@ -5262,7 +5261,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
         <v>67</v>
       </c>
@@ -5309,7 +5308,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>57</v>
       </c>
@@ -5354,7 +5353,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>71</v>
       </c>
@@ -5403,7 +5402,7 @@
       <c r="P54" s="16"/>
       <c r="Q54" s="16"/>
     </row>
-    <row r="55" spans="1:17" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>72</v>
       </c>
@@ -5446,7 +5445,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>74</v>
       </c>
@@ -5497,7 +5496,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
         <v>76</v>
       </c>
@@ -5540,7 +5539,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>76</v>
       </c>
@@ -5585,7 +5584,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>79</v>
       </c>
@@ -5630,7 +5629,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>81</v>
       </c>
@@ -5677,7 +5676,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>81</v>
       </c>
@@ -5720,7 +5719,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>51</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="170" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="170" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>84</v>
       </c>
@@ -5814,7 +5813,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>86</v>
       </c>
@@ -5857,7 +5856,7 @@
       <c r="P64" s="16"/>
       <c r="Q64" s="16"/>
     </row>
-    <row r="65" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>90</v>
       </c>
@@ -5902,7 +5901,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>90</v>
       </c>
@@ -5951,7 +5950,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>101</v>
       </c>
@@ -5998,7 +5997,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>393</v>
       </c>
@@ -6045,7 +6044,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>279</v>
       </c>
@@ -6088,7 +6087,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>281</v>
       </c>
@@ -6133,7 +6132,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>283</v>
       </c>
@@ -6156,7 +6155,7 @@
       <c r="P71" s="6"/>
       <c r="Q71" s="6"/>
     </row>
-    <row r="72" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>284</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>286</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>288</v>
       </c>
@@ -6287,7 +6286,7 @@
       <c r="P74" s="6"/>
       <c r="Q74" s="6"/>
     </row>
-    <row r="75" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>290</v>
       </c>
@@ -6324,7 +6323,7 @@
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
     </row>
-    <row r="76" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>292</v>
       </c>
@@ -6373,7 +6372,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>292</v>
       </c>
@@ -6420,7 +6419,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="221" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="221" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>86</v>
       </c>
@@ -6469,7 +6468,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>86</v>
       </c>
@@ -6515,7 +6514,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>297</v>
       </c>
@@ -6562,7 +6561,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>299</v>
       </c>
@@ -6611,7 +6610,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="255" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" ht="255" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>302</v>
       </c>
@@ -6660,7 +6659,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>303</v>
       </c>
@@ -6707,7 +6706,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>303</v>
       </c>
@@ -6752,7 +6751,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>306</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>308</v>
       </c>
@@ -6848,7 +6847,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="153" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>310</v>
       </c>
@@ -6899,7 +6898,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>313</v>
       </c>
@@ -6944,7 +6943,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>313</v>
       </c>
@@ -6989,7 +6988,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
         <v>315</v>
       </c>
@@ -7036,7 +7035,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="25" t="s">
         <v>317</v>
       </c>
@@ -7073,7 +7072,7 @@
       <c r="P91" s="6"/>
       <c r="Q91" s="6"/>
     </row>
-    <row r="92" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>323</v>
       </c>
@@ -7118,7 +7117,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>57</v>
       </c>
@@ -7161,7 +7160,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>320</v>
       </c>
@@ -7203,7 +7202,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="32" t="s">
         <v>324</v>
       </c>
@@ -7240,7 +7239,7 @@
       <c r="P95" s="6"/>
       <c r="Q95" s="6"/>
     </row>
-    <row r="96" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A96" s="32" t="s">
         <v>324</v>
       </c>
@@ -7283,7 +7282,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A97" s="32" t="s">
         <v>327</v>
       </c>
@@ -7328,7 +7327,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="170" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" ht="170" x14ac:dyDescent="0.2">
       <c r="A98" s="32" t="s">
         <v>327</v>
       </c>
@@ -7373,7 +7372,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A99" s="32" t="s">
         <v>329</v>
       </c>
@@ -7422,7 +7421,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A100" s="32" t="s">
         <v>331</v>
       </c>
@@ -7467,7 +7466,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="32" t="s">
         <v>333</v>
       </c>
@@ -7512,7 +7511,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="32" t="s">
         <v>335</v>
       </c>
@@ -7559,7 +7558,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A103" s="32" t="s">
         <v>337</v>
       </c>
@@ -7604,7 +7603,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" ht="68" x14ac:dyDescent="0.2">
       <c r="A104" s="32" t="s">
         <v>337</v>
       </c>
@@ -7651,7 +7650,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="153" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A105" s="32" t="s">
         <v>337</v>
       </c>
@@ -7700,7 +7699,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" s="32" t="s">
         <v>337</v>
       </c>
@@ -7743,7 +7742,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" ht="119" x14ac:dyDescent="0.2">
       <c r="A107" s="32" t="s">
         <v>343</v>
       </c>
@@ -7790,7 +7789,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="32" t="s">
         <v>344</v>
       </c>
@@ -7837,7 +7836,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="32" t="s">
         <v>346</v>
       </c>
@@ -7884,7 +7883,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="32" t="s">
         <v>346</v>
       </c>
@@ -7929,7 +7928,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="32" t="s">
         <v>349</v>
       </c>
@@ -7976,7 +7975,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="32" t="s">
         <v>350</v>
       </c>
@@ -8023,7 +8022,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="32" t="s">
         <v>350</v>
       </c>
@@ -8068,7 +8067,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="32" t="s">
         <v>353</v>
       </c>
@@ -8111,7 +8110,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="32" t="s">
         <v>355</v>
       </c>
@@ -8154,7 +8153,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="32" t="s">
         <v>357</v>
       </c>
@@ -8191,7 +8190,7 @@
       <c r="P116" s="6"/>
       <c r="Q116" s="6"/>
     </row>
-    <row r="117" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A117" s="31" t="s">
         <v>359</v>
       </c>
@@ -8238,7 +8237,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="32" t="s">
         <v>361</v>
       </c>
@@ -8281,7 +8280,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="32" t="s">
         <v>363</v>
       </c>
@@ -8328,7 +8327,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="32" t="s">
         <v>365</v>
       </c>
@@ -8379,7 +8378,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="32" t="s">
         <v>367</v>
       </c>
@@ -8424,7 +8423,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="122" spans="1:17" ht="153" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A122" s="32" t="s">
         <v>66</v>
       </c>
@@ -8475,7 +8474,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A123" s="32" t="s">
         <v>370</v>
       </c>
@@ -8524,7 +8523,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="32" t="s">
         <v>370</v>
       </c>
@@ -8571,7 +8570,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>437</v>
       </c>
@@ -8622,7 +8621,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="126" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>439</v>
       </c>
@@ -8673,7 +8672,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>521</v>
       </c>
@@ -8707,7 +8706,7 @@
       <c r="P127" s="6"/>
       <c r="Q127" s="6"/>
     </row>
-    <row r="128" spans="1:17" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" ht="102" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>523</v>
       </c>
@@ -8750,7 +8749,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="129" spans="1:17" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>531</v>
       </c>
@@ -8795,7 +8794,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="130" spans="1:17" ht="153" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" ht="153" x14ac:dyDescent="0.2">
       <c r="A130" s="34" t="s">
         <v>393</v>
       </c>
@@ -8844,7 +8843,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" ht="85" x14ac:dyDescent="0.2">
       <c r="A131" s="34" t="s">
         <v>538</v>
       </c>
@@ -8933,13 +8932,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R131" xr:uid="{42D43BBC-FD48-6D4B-B79D-D054E095EE14}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="12844"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R131" xr:uid="{42D43BBC-FD48-6D4B-B79D-D054E095EE14}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>